<commit_message>
Completed writing to xlsx file
</commit_message>
<xml_diff>
--- a/Detailed Player info.xlsx
+++ b/Detailed Player info.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+  <si>
+    <t>Created On:</t>
+  </si>
+  <si>
+    <t>27/10/2020 15:09</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
@@ -41,6 +47,63 @@
   </si>
   <si>
     <t>Rss Assist</t>
+  </si>
+  <si>
+    <t>Name Image</t>
+  </si>
+  <si>
+    <t>Kaisa</t>
+  </si>
+  <si>
+    <t>18110974</t>
+  </si>
+  <si>
+    <t>HOF</t>
+  </si>
+  <si>
+    <t>361591432</t>
+  </si>
+  <si>
+    <t>538509090</t>
+  </si>
+  <si>
+    <t>235819159</t>
+  </si>
+  <si>
+    <t>59038305</t>
+  </si>
+  <si>
+    <t>30009212</t>
+  </si>
+  <si>
+    <t>6585660615</t>
+  </si>
+  <si>
+    <t>별 빠따 | 541</t>
+  </si>
+  <si>
+    <t>39413819</t>
+  </si>
+  <si>
+    <t>Thes</t>
+  </si>
+  <si>
+    <t>70633255</t>
+  </si>
+  <si>
+    <t>1029330</t>
+  </si>
+  <si>
+    <t>659165</t>
+  </si>
+  <si>
+    <t>178959</t>
+  </si>
+  <si>
+    <t>3467284</t>
+  </si>
+  <si>
+    <t>819649729</t>
   </si>
 </sst>
 </file>
@@ -94,6 +157,87 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="1-name.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="381000"/>
+          <a:ext cx="1362075" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="2-name.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="571500"/>
+          <a:ext cx="1362075" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -381,42 +525,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated screenshot.py to capture first 3 players. Updated ocr.py to goto correct directory for the images
</commit_message>
<xml_diff>
--- a/Detailed Player info.xlsx
+++ b/Detailed Player info.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
   <si>
     <t>Created On:</t>
   </si>
   <si>
-    <t>27/10/2020 15:09</t>
+    <t>27/10/2020 15:54</t>
   </si>
   <si>
     <t>Name</t>
@@ -61,7 +61,7 @@
     <t>HOF</t>
   </si>
   <si>
-    <t>361591432</t>
+    <t>361623432</t>
   </si>
   <si>
     <t>538509090</t>
@@ -79,31 +79,229 @@
     <t>6585660615</t>
   </si>
   <si>
-    <t>별 빠따 | 541</t>
-  </si>
-  <si>
-    <t>39413819</t>
-  </si>
-  <si>
-    <t>Thes</t>
-  </si>
-  <si>
-    <t>70633255</t>
-  </si>
-  <si>
-    <t>1029330</t>
-  </si>
-  <si>
-    <t>659165</t>
-  </si>
-  <si>
-    <t>178959</t>
-  </si>
-  <si>
-    <t>3467284</t>
-  </si>
-  <si>
-    <t>819649729</t>
+    <t>Carpenter Force</t>
+  </si>
+  <si>
+    <t>43209419</t>
+  </si>
+  <si>
+    <t>KrU</t>
+  </si>
+  <si>
+    <t>140927349</t>
+  </si>
+  <si>
+    <t>136998792</t>
+  </si>
+  <si>
+    <t>109085851</t>
+  </si>
+  <si>
+    <t>10627690</t>
+  </si>
+  <si>
+    <t>2409418</t>
+  </si>
+  <si>
+    <t>929772451</t>
+  </si>
+  <si>
+    <t>Lady PICO</t>
+  </si>
+  <si>
+    <t>43173244</t>
+  </si>
+  <si>
+    <t>HOE</t>
+  </si>
+  <si>
+    <t>112453745</t>
+  </si>
+  <si>
+    <t>24704610</t>
+  </si>
+  <si>
+    <t>8581036</t>
+  </si>
+  <si>
+    <t>5003771</t>
+  </si>
+  <si>
+    <t>1925817</t>
+  </si>
+  <si>
+    <t>1417392279</t>
+  </si>
+  <si>
+    <t>MiS7RaL</t>
+  </si>
+  <si>
+    <t>7688876</t>
+  </si>
+  <si>
+    <t>104389920</t>
+  </si>
+  <si>
+    <t>67750051</t>
+  </si>
+  <si>
+    <t>27680727</t>
+  </si>
+  <si>
+    <t>4829669</t>
+  </si>
+  <si>
+    <t>2590395</t>
+  </si>
+  <si>
+    <t>2089845089</t>
+  </si>
+  <si>
+    <t>Uggabuggalll</t>
+  </si>
+  <si>
+    <t>17015565</t>
+  </si>
+  <si>
+    <t>103282076</t>
+  </si>
+  <si>
+    <t>9178258</t>
+  </si>
+  <si>
+    <t>17207953</t>
+  </si>
+  <si>
+    <t>9761304</t>
+  </si>
+  <si>
+    <t>1148769</t>
+  </si>
+  <si>
+    <t>1981358317</t>
+  </si>
+  <si>
+    <t>King Boogie</t>
+  </si>
+  <si>
+    <t>17156102</t>
+  </si>
+  <si>
+    <t>101921907</t>
+  </si>
+  <si>
+    <t>52625585</t>
+  </si>
+  <si>
+    <t>18725998</t>
+  </si>
+  <si>
+    <t>11461374</t>
+  </si>
+  <si>
+    <t>2398137</t>
+  </si>
+  <si>
+    <t>288307518</t>
+  </si>
+  <si>
+    <t>할리퀸 04660</t>
+  </si>
+  <si>
+    <t>120247</t>
+  </si>
+  <si>
+    <t>100676136</t>
+  </si>
+  <si>
+    <t>152816628</t>
+  </si>
+  <si>
+    <t>48923743</t>
+  </si>
+  <si>
+    <t>10772629</t>
+  </si>
+  <si>
+    <t>5997098</t>
+  </si>
+  <si>
+    <t>4394203487</t>
+  </si>
+  <si>
+    <t>chop stick</t>
+  </si>
+  <si>
+    <t>4319801</t>
+  </si>
+  <si>
+    <t>ByuL</t>
+  </si>
+  <si>
+    <t>100472434</t>
+  </si>
+  <si>
+    <t>26833508</t>
+  </si>
+  <si>
+    <t>3677215</t>
+  </si>
+  <si>
+    <t>187619</t>
+  </si>
+  <si>
+    <t>2892267</t>
+  </si>
+  <si>
+    <t>4314980947</t>
+  </si>
+  <si>
+    <t>이성계</t>
+  </si>
+  <si>
+    <t>17029446</t>
+  </si>
+  <si>
+    <t>100305640</t>
+  </si>
+  <si>
+    <t>183394851</t>
+  </si>
+  <si>
+    <t>91825412</t>
+  </si>
+  <si>
+    <t>8778795</t>
+  </si>
+  <si>
+    <t>6180642</t>
+  </si>
+  <si>
+    <t>3365246332</t>
+  </si>
+  <si>
+    <t>KaidenLeon</t>
+  </si>
+  <si>
+    <t>7670406</t>
+  </si>
+  <si>
+    <t>100180369</t>
+  </si>
+  <si>
+    <t>170358299</t>
+  </si>
+  <si>
+    <t>44849619</t>
+  </si>
+  <si>
+    <t>14335088</t>
+  </si>
+  <si>
+    <t>4986532</t>
+  </si>
+  <si>
+    <t>4036887250</t>
   </si>
 </sst>
 </file>
@@ -228,6 +426,310 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5486400" y="571500"/>
+          <a:ext cx="1362075" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="3-name.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="762000"/>
+          <a:ext cx="1362075" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="4-name.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="952500"/>
+          <a:ext cx="1362075" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="5-name.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="1143000"/>
+          <a:ext cx="1362075" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="6-name.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="1333500"/>
+          <a:ext cx="1362075" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="7-name.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="1524000"/>
+          <a:ext cx="1362075" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="8-name.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="1714500"/>
+          <a:ext cx="1362075" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="9-name.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="1905000"/>
+          <a:ext cx="1362075" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="10-name.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="2095500"/>
           <a:ext cx="1362075" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -525,7 +1027,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -629,6 +1131,238 @@
         <v>29</v>
       </c>
     </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>